<commit_message>
Run sex DE per cell type within VMH, ARC domains defined using Yi's parameters, smoothing all 5 ARC clusters or the 3 of them that dont extend to periventricular area (and their paired, competitively labeled VMH domain counterparts), and sex DE agnostic to cell type within those two sets of domain assignments
</commit_message>
<xml_diff>
--- a/xenium_HYP/processed-data/05_Banksy_M0lam0_res2_multisamp/02-M0l0kg6_topClusMarkers_celltypes_annotated.xlsx
+++ b/xenium_HYP/processed-data/05_Banksy_M0lam0_res2_multisamp/02-M0l0kg6_topClusMarkers_celltypes_annotated.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmulvey/Desktop/KM Lab/local_hthspatial/xenium_HYP/processed-data/05_Banksy_M0lam0_res2_multisamp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6C8F5A6C-D8F7-D14A-B2A5-8409F6B3295A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4190B60C-5D4D-B342-B9FF-CAE03FA2D8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="2320" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="10760" yWindow="2320" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="02-M0l0kg6_topClusMarkers" sheetId="1" r:id="rId1"/>
@@ -1303,7 +1303,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2141,11 +2141,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2801"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2709" workbookViewId="0">
-      <selection activeCell="F2727" sqref="F2727:F2785"/>
+    <sheetView tabSelected="1" topLeftCell="A906" workbookViewId="0">
+      <selection activeCell="E921" sqref="E921"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18285,7 +18285,7 @@
         <v>0.59118350101864903</v>
       </c>
       <c r="E912" t="s">
-        <v>388</v>
+        <v>413</v>
       </c>
     </row>
     <row r="913" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>